<commit_message>
ajoute de l'itération 1
</commit_message>
<xml_diff>
--- a/estimation.xlsx
+++ b/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -138,6 +138,57 @@
   </si>
   <si>
     <t xml:space="preserve">utiliser plus de commande qui sont généré aléatoirement </t>
+  </si>
+  <si>
+    <t>30-01-2017</t>
+  </si>
+  <si>
+    <t>31-01-2017</t>
+  </si>
+  <si>
+    <t>06-02-2017</t>
+  </si>
+  <si>
+    <t>07-02-2017</t>
+  </si>
+  <si>
+    <t>13-02-2017</t>
+  </si>
+  <si>
+    <t>14-02-2017</t>
+  </si>
+  <si>
+    <t>Recherche sur les fragmented activity, plus tutoriel</t>
+  </si>
+  <si>
+    <t>tentative de faire fonctionner les fragmented activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser mon cellulaire pour faire foncitonner mon app </t>
+  </si>
+  <si>
+    <t xml:space="preserve">suppresion des fragmented activity et utilisation des gridview </t>
+  </si>
+  <si>
+    <t>erreur avec les gridview commencement avec les layout</t>
+  </si>
+  <si>
+    <t>travaille sur l'interface  et configuration des bouton pour activé le  Clicke</t>
+  </si>
+  <si>
+    <t>02-02-2017</t>
+  </si>
+  <si>
+    <t>modification des fragments et essaie d'autres tuto</t>
+  </si>
+  <si>
+    <t>18-02-2017</t>
+  </si>
+  <si>
+    <t>recherche pour faire un timer et modification du theme</t>
+  </si>
+  <si>
+    <t>J'ai mal gerer mon temps mais je suis tout de même satisfait, plusieurs tentative pour faire l'interface qui n'on pas fonctionné. Parcontre je n'ai pas respecter mon itinéraire, j'ai noter que je devais faire l'interface a la fin mais je n'avais pas réfléchit au fait qu'il me faut des objet sur lequel progguer.</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -1821,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1879,44 +1930,92 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
+      <c r="A21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
@@ -2000,7 +2099,7 @@
       <c r="B37" s="19"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2013,7 +2112,9 @@
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
@@ -2022,7 +2123,9 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="21"/>

</xml_diff>